<commit_message>
"created getTrace controller and route for battery_id "
</commit_message>
<xml_diff>
--- a/static/end_of_line.xlsx
+++ b/static/end_of_line.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\000_WORKING\Godrej_product_tracibility\docker_images\mysql-image\backend\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B48AC55-CCC0-4500-8E8A-8B26B6865BD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD212960-0EAF-4776-8453-F02DDC6AFA39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="3420" windowWidth="23256" windowHeight="12456" xr2:uid="{EB4617D1-40C9-427E-B8CB-7EE6D6D9ACF3}"/>
+    <workbookView xWindow="-23148" yWindow="2880" windowWidth="23256" windowHeight="12456" xr2:uid="{EB4617D1-40C9-427E-B8CB-7EE6D6D9ACF3}"/>
   </bookViews>
   <sheets>
     <sheet name="end_of_line" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="111">
   <si>
     <t>Format for uploading battery parameters from End of line PLC</t>
   </si>
@@ -360,6 +360,15 @@
   </si>
   <si>
     <t>ACELL0104</t>
+  </si>
+  <si>
+    <t>testing_timestamp</t>
+  </si>
+  <si>
+    <t>2020-05-19 01:00:00</t>
+  </si>
+  <si>
+    <t>2020-05-19 01:30:00</t>
   </si>
 </sst>
 </file>
@@ -389,7 +398,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -425,18 +434,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -771,10 +824,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E6106C7-55B1-468C-86B3-D158BE651907}">
-  <dimension ref="A1:G92"/>
+  <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B92"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B78" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,44 +841,49 @@
     <col min="4" max="4" width="15.5703125" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="30" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -841,11 +902,14 @@
       <c r="F3">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G3" s="3">
-        <v>45669</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -864,11 +928,14 @@
       <c r="F4">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G4" s="3">
-        <v>45669</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -887,11 +954,14 @@
       <c r="F5">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G5" s="3">
-        <v>45669</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -910,11 +980,14 @@
       <c r="F6">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G6" s="3">
-        <v>45669</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G6" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -933,11 +1006,14 @@
       <c r="F7">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G7" s="3">
-        <v>45669</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -956,11 +1032,14 @@
       <c r="F8">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G8" s="3">
-        <v>45669</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -979,11 +1058,14 @@
       <c r="F9">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G9" s="3">
-        <v>45669</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G9" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1002,11 +1084,14 @@
       <c r="F10">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G10" s="3">
-        <v>45669</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G10" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1025,11 +1110,14 @@
       <c r="F11">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G11" s="3">
-        <v>45669</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G11" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1048,11 +1136,14 @@
       <c r="F12">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G12" s="3">
-        <v>45669</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G12" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1071,11 +1162,14 @@
       <c r="F13">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G13" s="3">
-        <v>45670</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1094,11 +1188,14 @@
       <c r="F14">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G14" s="3">
-        <v>45670</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G14" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1117,11 +1214,14 @@
       <c r="F15">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G15" s="3">
-        <v>45670</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G15" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1140,11 +1240,14 @@
       <c r="F16">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G16" s="3">
-        <v>45670</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G16" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1163,11 +1266,14 @@
       <c r="F17">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G17" s="3">
-        <v>45670</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1186,11 +1292,14 @@
       <c r="F18">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G18" s="3">
-        <v>45670</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1209,11 +1318,14 @@
       <c r="F19">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G19" s="3">
-        <v>45670</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -1232,11 +1344,14 @@
       <c r="F20">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G20" s="3">
-        <v>45670</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G20" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1255,11 +1370,14 @@
       <c r="F21">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G21" s="3">
-        <v>45671</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G21" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -1278,11 +1396,14 @@
       <c r="F22">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G22" s="3">
-        <v>45672</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G22" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -1301,11 +1422,14 @@
       <c r="F23">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G23" s="3">
-        <v>45673</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -1324,11 +1448,14 @@
       <c r="F24">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G24" s="3">
-        <v>45674</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G24" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -1347,11 +1474,14 @@
       <c r="F25">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G25" s="3">
-        <v>45675</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G25" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -1370,11 +1500,14 @@
       <c r="F26">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G26" s="3">
-        <v>45676</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G26" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -1393,11 +1526,14 @@
       <c r="F27">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G27" s="3">
-        <v>45677</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G27" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -1416,11 +1552,14 @@
       <c r="F28">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G28" s="3">
-        <v>45678</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G28" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -1439,11 +1578,14 @@
       <c r="F29">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G29" s="3">
-        <v>45679</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G29" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>11</v>
       </c>
@@ -1462,11 +1604,14 @@
       <c r="F30">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G30" s="3">
-        <v>45680</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G30" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>11</v>
       </c>
@@ -1485,11 +1630,14 @@
       <c r="F31">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G31" s="3">
-        <v>45681</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G31" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>11</v>
       </c>
@@ -1508,11 +1656,14 @@
       <c r="F32">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G32" s="3">
-        <v>45682</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G32" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -1531,11 +1682,14 @@
       <c r="F33">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G33" s="3">
-        <v>45683</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G33" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -1554,11 +1708,14 @@
       <c r="F34">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G34" s="3">
-        <v>45684</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G34" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -1577,11 +1734,14 @@
       <c r="F35">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G35" s="3">
-        <v>45685</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G35" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -1600,11 +1760,14 @@
       <c r="F36">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G36" s="3">
-        <v>45686</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G36" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -1623,11 +1786,14 @@
       <c r="F37">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G37" s="3">
-        <v>45687</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G37" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -1646,11 +1812,14 @@
       <c r="F38">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G38" s="3">
-        <v>45688</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G38" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -1669,11 +1838,14 @@
       <c r="F39">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G39" s="3">
-        <v>45689</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G39" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>12</v>
       </c>
@@ -1692,11 +1864,14 @@
       <c r="F40">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G40" s="3">
-        <v>45690</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G40" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -1715,11 +1890,14 @@
       <c r="F41">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G41" s="3">
-        <v>45691</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G41" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -1738,11 +1916,14 @@
       <c r="F42">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G42" s="3">
-        <v>45692</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G42" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H42" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -1761,11 +1942,14 @@
       <c r="F43">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G43" s="3">
-        <v>45693</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G43" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -1784,11 +1968,14 @@
       <c r="F44">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G44" s="3">
-        <v>45694</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G44" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -1807,11 +1994,14 @@
       <c r="F45">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G45" s="3">
-        <v>45695</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G45" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -1830,11 +2020,14 @@
       <c r="F46">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G46" s="3">
-        <v>45696</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G46" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H46" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>12</v>
       </c>
@@ -1853,11 +2046,14 @@
       <c r="F47">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G47" s="3">
-        <v>45697</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G47" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>13</v>
       </c>
@@ -1876,11 +2072,14 @@
       <c r="F48">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G48" s="3">
-        <v>45698</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G48" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H48" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>13</v>
       </c>
@@ -1899,11 +2098,14 @@
       <c r="F49">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G49" s="3">
-        <v>45699</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G49" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H49" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>13</v>
       </c>
@@ -1922,11 +2124,14 @@
       <c r="F50">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G50" s="3">
-        <v>45700</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G50" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H50" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>13</v>
       </c>
@@ -1945,11 +2150,14 @@
       <c r="F51">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G51" s="3">
-        <v>45701</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G51" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H51" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>13</v>
       </c>
@@ -1968,11 +2176,14 @@
       <c r="F52">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G52" s="3">
-        <v>45702</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G52" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H52" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>13</v>
       </c>
@@ -1991,11 +2202,14 @@
       <c r="F53">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G53" s="3">
-        <v>45703</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G53" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H53" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>13</v>
       </c>
@@ -2014,11 +2228,14 @@
       <c r="F54">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G54" s="3">
-        <v>45704</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G54" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H54" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>13</v>
       </c>
@@ -2037,11 +2254,14 @@
       <c r="F55">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G55" s="3">
-        <v>45705</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G55" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H55" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>13</v>
       </c>
@@ -2060,11 +2280,14 @@
       <c r="F56">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G56" s="3">
-        <v>45706</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G56" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H56" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>14</v>
       </c>
@@ -2083,11 +2306,14 @@
       <c r="F57">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G57" s="3">
-        <v>45707</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G57" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H57" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>14</v>
       </c>
@@ -2106,11 +2332,14 @@
       <c r="F58">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G58" s="3">
-        <v>45708</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G58" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H58" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>14</v>
       </c>
@@ -2129,11 +2358,14 @@
       <c r="F59">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G59" s="3">
-        <v>45709</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G59" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H59" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>14</v>
       </c>
@@ -2152,11 +2384,14 @@
       <c r="F60">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G60" s="3">
-        <v>45710</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G60" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H60" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>14</v>
       </c>
@@ -2175,11 +2410,14 @@
       <c r="F61">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G61" s="3">
-        <v>45711</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G61" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H61" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -2198,11 +2436,14 @@
       <c r="F62">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G62" s="3">
-        <v>45712</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G62" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H62" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -2221,11 +2462,14 @@
       <c r="F63">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G63" s="3">
-        <v>45713</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G63" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H63" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>14</v>
       </c>
@@ -2244,11 +2488,14 @@
       <c r="F64">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G64" s="3">
-        <v>45714</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G64" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H64" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>14</v>
       </c>
@@ -2267,11 +2514,14 @@
       <c r="F65">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G65" s="3">
-        <v>45715</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G65" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H65" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>15</v>
       </c>
@@ -2290,11 +2540,14 @@
       <c r="F66">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G66" s="3">
-        <v>45716</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G66" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H66" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>15</v>
       </c>
@@ -2313,11 +2566,14 @@
       <c r="F67">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G67" s="3">
-        <v>45717</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G67" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H67" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>15</v>
       </c>
@@ -2336,11 +2592,14 @@
       <c r="F68">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G68" s="3">
-        <v>45718</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G68" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H68" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>15</v>
       </c>
@@ -2359,11 +2618,14 @@
       <c r="F69">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G69" s="3">
-        <v>45719</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G69" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H69" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>15</v>
       </c>
@@ -2382,11 +2644,14 @@
       <c r="F70">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G70" s="3">
-        <v>45720</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G70" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H70" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>15</v>
       </c>
@@ -2405,11 +2670,14 @@
       <c r="F71">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G71" s="3">
-        <v>45721</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G71" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H71" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>15</v>
       </c>
@@ -2428,11 +2696,14 @@
       <c r="F72">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G72" s="3">
-        <v>45722</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G72" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H72" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>15</v>
       </c>
@@ -2451,11 +2722,14 @@
       <c r="F73">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G73" s="3">
-        <v>45723</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G73" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H73" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>15</v>
       </c>
@@ -2474,11 +2748,14 @@
       <c r="F74">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G74" s="3">
-        <v>45724</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G74" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H74" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>17</v>
       </c>
@@ -2497,11 +2774,14 @@
       <c r="F75">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G75" s="3">
-        <v>45725</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G75" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H75" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>17</v>
       </c>
@@ -2520,11 +2800,14 @@
       <c r="F76">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G76" s="3">
-        <v>45726</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G76" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H76" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>17</v>
       </c>
@@ -2543,11 +2826,14 @@
       <c r="F77">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G77" s="3">
-        <v>45727</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G77" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H77" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>17</v>
       </c>
@@ -2566,11 +2852,14 @@
       <c r="F78">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G78" s="3">
-        <v>45728</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G78" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H78" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>17</v>
       </c>
@@ -2589,11 +2878,14 @@
       <c r="F79">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G79" s="3">
-        <v>45729</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G79" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H79" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>17</v>
       </c>
@@ -2612,11 +2904,14 @@
       <c r="F80">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G80" s="3">
-        <v>45730</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G80" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H80" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>17</v>
       </c>
@@ -2635,11 +2930,14 @@
       <c r="F81">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G81" s="3">
-        <v>45731</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G81" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H81" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>17</v>
       </c>
@@ -2658,11 +2956,14 @@
       <c r="F82">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G82" s="3">
-        <v>45732</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G82" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H82" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>17</v>
       </c>
@@ -2681,11 +2982,14 @@
       <c r="F83">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G83" s="3">
-        <v>45733</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G83" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H83" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>16</v>
       </c>
@@ -2704,11 +3008,14 @@
       <c r="F84">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G84" s="3">
-        <v>45734</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G84" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H84" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>16</v>
       </c>
@@ -2727,11 +3034,14 @@
       <c r="F85">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G85" s="3">
-        <v>45735</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G85" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H85" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>16</v>
       </c>
@@ -2750,11 +3060,14 @@
       <c r="F86">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G86" s="3">
-        <v>45736</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G86" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H86" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>16</v>
       </c>
@@ -2773,11 +3086,14 @@
       <c r="F87">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G87" s="3">
-        <v>45737</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G87" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H87" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>16</v>
       </c>
@@ -2796,11 +3112,14 @@
       <c r="F88">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G88" s="3">
-        <v>45738</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G88" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H88" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>16</v>
       </c>
@@ -2819,11 +3138,14 @@
       <c r="F89">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G89" s="3">
-        <v>45739</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G89" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H89" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>16</v>
       </c>
@@ -2842,11 +3164,14 @@
       <c r="F90">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G90" s="3">
-        <v>45740</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G90" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H90" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>16</v>
       </c>
@@ -2865,11 +3190,14 @@
       <c r="F91">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G91" s="3">
-        <v>45741</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G91" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H91" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>16</v>
       </c>
@@ -2888,13 +3216,16 @@
       <c r="F92">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G92" s="3">
-        <v>45742</v>
+      <c r="G92" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H92" s="7" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>